<commit_message>
I think the Bracket is finished
</commit_message>
<xml_diff>
--- a/March Madness/March Madness 2022/ResultsAndRankings21.xlsx
+++ b/March Madness/March Madness 2022/ResultsAndRankings21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daddy\Documents\R\MyProjects\March Madness\March Madness 2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCC9AFA-7E50-4246-98B6-310A66B25C26}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5581FF7-FAE9-4867-B439-F3BE7D0AD7AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6995" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7016" uniqueCount="321">
   <si>
     <t>Date</t>
   </si>
@@ -1355,11 +1355,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2312"/>
+  <dimension ref="A1:K2319"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2186" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q2197" sqref="Q2197"/>
+      <pane ySplit="1" topLeftCell="A2294" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I2316" sqref="I2316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -82291,6 +82291,251 @@
         <v>46</v>
       </c>
     </row>
+    <row r="2313" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2313" s="1">
+        <v>44285</v>
+      </c>
+      <c r="B2313">
+        <v>2021</v>
+      </c>
+      <c r="C2313">
+        <v>4</v>
+      </c>
+      <c r="D2313" t="s">
+        <v>306</v>
+      </c>
+      <c r="E2313">
+        <v>57</v>
+      </c>
+      <c r="F2313">
+        <v>1</v>
+      </c>
+      <c r="G2313" t="s">
+        <v>206</v>
+      </c>
+      <c r="H2313">
+        <v>85</v>
+      </c>
+      <c r="I2313">
+        <v>6</v>
+      </c>
+      <c r="J2313" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2313">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2314" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2314" s="1">
+        <v>44285</v>
+      </c>
+      <c r="B2314">
+        <v>2021</v>
+      </c>
+      <c r="C2314">
+        <v>4</v>
+      </c>
+      <c r="D2314" t="s">
+        <v>305</v>
+      </c>
+      <c r="E2314">
+        <v>58</v>
+      </c>
+      <c r="F2314">
+        <v>11</v>
+      </c>
+      <c r="G2314" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2314">
+        <v>51</v>
+      </c>
+      <c r="I2314">
+        <v>1</v>
+      </c>
+      <c r="J2314" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2314">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2315" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2315" s="1">
+        <v>44285</v>
+      </c>
+      <c r="B2315">
+        <v>2021</v>
+      </c>
+      <c r="C2315">
+        <v>4</v>
+      </c>
+      <c r="D2315" t="s">
+        <v>307</v>
+      </c>
+      <c r="E2315">
+        <v>59</v>
+      </c>
+      <c r="F2315">
+        <v>1</v>
+      </c>
+      <c r="G2315" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2315">
+        <v>81</v>
+      </c>
+      <c r="I2315">
+        <v>3</v>
+      </c>
+      <c r="J2315" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2315">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2316" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2316" s="1">
+        <v>44285</v>
+      </c>
+      <c r="B2316">
+        <v>2021</v>
+      </c>
+      <c r="C2316">
+        <v>4</v>
+      </c>
+      <c r="D2316" t="s">
+        <v>309</v>
+      </c>
+      <c r="E2316">
+        <v>60</v>
+      </c>
+      <c r="F2316">
+        <v>2</v>
+      </c>
+      <c r="G2316" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2316">
+        <v>67</v>
+      </c>
+      <c r="I2316">
+        <v>12</v>
+      </c>
+      <c r="J2316" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2316">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2317" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2317" s="1">
+        <v>44289</v>
+      </c>
+      <c r="B2317">
+        <v>2021</v>
+      </c>
+      <c r="C2317">
+        <v>5</v>
+      </c>
+      <c r="D2317" t="s">
+        <v>315</v>
+      </c>
+      <c r="E2317">
+        <v>61</v>
+      </c>
+      <c r="F2317">
+        <v>1</v>
+      </c>
+      <c r="G2317" t="s">
+        <v>206</v>
+      </c>
+      <c r="H2317">
+        <v>93</v>
+      </c>
+      <c r="I2317">
+        <v>11</v>
+      </c>
+      <c r="J2317" t="s">
+        <v>103</v>
+      </c>
+      <c r="K2317">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2318" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2318" s="1">
+        <v>44289</v>
+      </c>
+      <c r="B2318">
+        <v>2021</v>
+      </c>
+      <c r="C2318">
+        <v>5</v>
+      </c>
+      <c r="D2318" t="s">
+        <v>315</v>
+      </c>
+      <c r="E2318">
+        <v>62</v>
+      </c>
+      <c r="F2318">
+        <v>1</v>
+      </c>
+      <c r="G2318" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2318">
+        <v>78</v>
+      </c>
+      <c r="I2318">
+        <v>2</v>
+      </c>
+      <c r="J2318" t="s">
+        <v>112</v>
+      </c>
+      <c r="K2318">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2319" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2319" s="1">
+        <v>44291</v>
+      </c>
+      <c r="B2319">
+        <v>2021</v>
+      </c>
+      <c r="C2319">
+        <v>6</v>
+      </c>
+      <c r="D2319" t="s">
+        <v>316</v>
+      </c>
+      <c r="E2319">
+        <v>63</v>
+      </c>
+      <c r="F2319">
+        <v>1</v>
+      </c>
+      <c r="G2319" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2319">
+        <v>86</v>
+      </c>
+      <c r="I2319">
+        <v>1</v>
+      </c>
+      <c r="J2319" t="s">
+        <v>206</v>
+      </c>
+      <c r="K2319">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>